<commit_message>
Fix handPile order so category_content[0] is first card flipped
Converter now reverses handPile array so the first entry in the
spreadsheet category_content is the first card the player sees
when flipping. Also update regenerated level files and remove level_13.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/config/string_config.xlsx
+++ b/config/string_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bin/Documents/JoyCastle/claudeCode/solitaire-tile-bingo/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B0C8187-3A69-2E46-8B01-CAAEFFF41B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3359C9C0-CD02-174E-B00E-38CE62847162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3800" yWindow="4320" windowWidth="25440" windowHeight="13940" xr2:uid="{515064CD-50D1-F94A-A5CC-CC4734FE40F7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="1490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="1491">
   <si>
     <t>id</t>
   </si>
@@ -4504,6 +4504,10 @@
   </si>
   <si>
     <t>Landmass</t>
+  </si>
+  <si>
+    <t>Wardrobe</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4888,8 +4892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F719E73-D7BB-CA44-A0DE-4D5D8169EFF3}">
   <dimension ref="A1:C778"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A721" workbookViewId="0">
+      <selection activeCell="C734" sqref="C734"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11458,7 +11462,7 @@
       </c>
       <c r="B729" s="1"/>
       <c r="C729" s="1" t="s">
-        <v>210</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="730" spans="1:3">

</xml_diff>